<commit_message>
MR (raw and SPSS) corrections allowed now
</commit_message>
<xml_diff>
--- a/unit_testing/APA_tables/expected tables/57_spss_mr_allstats.xlsx
+++ b/unit_testing/APA_tables/expected tables/57_spss_mr_allstats.xlsx
@@ -377,7 +377,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -413,7 +413,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>pvalues</t>
+          <t>p</t>
         </is>
       </c>
     </row>
@@ -441,7 +441,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>.238</t>
+          <t>.401</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>.186</t>
+          <t>.401</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>.241</t>
+          <t>.401</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>.415</t>
+          <t>.519</t>
         </is>
       </c>
     </row>
@@ -584,6 +584,13 @@
       <c r="A8" t="inlineStr">
         <is>
           <t>Dependent variable: var5</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Multiple tests correction applied to p values: Benjamini-Hochberg</t>
         </is>
       </c>
     </row>

</xml_diff>